<commit_message>
Update Electricité de Strasbourg prices of 2026-02-01
</commit_message>
<xml_diff>
--- a/contracts/electricite-de-strasbourg/tarif-bleu-base/Option_Base.xlsx
+++ b/contracts/electricite-de-strasbourg/tarif-bleu-base/Option_Base.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="43">
   <si>
     <t xml:space="preserve">DATE_DEBUT</t>
   </si>
@@ -31,13 +31,10 @@
     <t xml:space="preserve">P_SOUSCRITE</t>
   </si>
   <si>
-    <t xml:space="preserve">PART_FIXE_HT</t>
+    <t xml:space="preserve">PART_FIXE_TTC_MOIS</t>
   </si>
   <si>
     <t xml:space="preserve">PART_FIXE_TTC</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PART_VARIABLE_HT</t>
   </si>
   <si>
     <t xml:space="preserve">PART_VARIABLE_TTC</t>
@@ -227,7 +224,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -237,10 +234,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -367,14 +360,14 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G101"/>
+  <dimension ref="A1:F101"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B65" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B77" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="A65" activeCellId="0" sqref="A65"/>
-      <selection pane="bottomRight" activeCell="B77" activeCellId="0" sqref="B77"/>
+      <selection pane="bottomLeft" activeCell="A77" activeCellId="0" sqref="A77"/>
+      <selection pane="bottomRight" activeCell="F94" activeCellId="0" sqref="F94"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -384,8 +377,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="14.03"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="14.62"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="13.41"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="19.35"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="20.45"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="20.45"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -407,16 +399,13 @@
       <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>6</v>
-      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>7</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>8</v>
       </c>
       <c r="C2" s="1" t="n">
         <v>3</v>
@@ -425,16 +414,16 @@
         <f aca="false">12*4.54</f>
         <v>54.48</v>
       </c>
-      <c r="G2" s="1" t="n">
+      <c r="F2" s="1" t="n">
         <v>0.1503</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>7</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>8</v>
       </c>
       <c r="C3" s="1" t="n">
         <v>6</v>
@@ -443,16 +432,16 @@
         <f aca="false">12*7.37</f>
         <v>88.44</v>
       </c>
-      <c r="G3" s="1" t="n">
+      <c r="F3" s="1" t="n">
         <v>0.1503</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>7</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>8</v>
       </c>
       <c r="C4" s="1" t="n">
         <v>9</v>
@@ -461,16 +450,16 @@
         <f aca="false">12*9.77</f>
         <v>117.24</v>
       </c>
-      <c r="G4" s="1" t="n">
+      <c r="F4" s="1" t="n">
         <v>0.1503</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>7</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>8</v>
       </c>
       <c r="C5" s="1" t="n">
         <v>12</v>
@@ -479,16 +468,16 @@
         <f aca="false">12*15.01</f>
         <v>180.12</v>
       </c>
-      <c r="G5" s="1" t="n">
+      <c r="F5" s="1" t="n">
         <v>0.1503</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="2" t="s">
         <v>7</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>8</v>
       </c>
       <c r="C6" s="1" t="n">
         <v>15</v>
@@ -497,506 +486,506 @@
         <f aca="false">12*17.21</f>
         <v>206.52</v>
       </c>
-      <c r="G6" s="1" t="n">
+      <c r="F6" s="1" t="n">
         <v>0.1503</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C7" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="G7" s="1" t="n">
+      <c r="F7" s="1" t="n">
         <v>0.1503</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C8" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="G8" s="1" t="n">
+      <c r="F8" s="1" t="n">
         <v>0.1503</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C9" s="1" t="n">
         <v>9</v>
       </c>
-      <c r="G9" s="1" t="n">
+      <c r="F9" s="1" t="n">
         <v>0.1503</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C10" s="1" t="n">
         <v>12</v>
       </c>
-      <c r="G10" s="1" t="n">
+      <c r="F10" s="1" t="n">
         <v>0.1503</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C11" s="1" t="n">
         <v>15</v>
       </c>
-      <c r="G11" s="1" t="n">
+      <c r="F11" s="1" t="n">
         <v>0.1503</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B12" s="2" t="s">
         <v>11</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>12</v>
       </c>
       <c r="C12" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="G12" s="1" t="n">
+      <c r="F12" s="1" t="n">
         <v>0.1546</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B13" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B13" s="2" t="s">
-        <v>12</v>
-      </c>
       <c r="C13" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="G13" s="1" t="n">
+      <c r="F13" s="1" t="n">
         <v>0.1466</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B14" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B14" s="2" t="s">
-        <v>12</v>
-      </c>
       <c r="C14" s="1" t="n">
         <v>9</v>
       </c>
-      <c r="G14" s="1" t="n">
+      <c r="F14" s="1" t="n">
         <v>0.1483</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B15" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B15" s="2" t="s">
-        <v>12</v>
-      </c>
       <c r="C15" s="1" t="n">
         <v>12</v>
       </c>
-      <c r="G15" s="1" t="n">
+      <c r="F15" s="1" t="n">
         <v>0.1483</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B16" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B16" s="2" t="s">
-        <v>12</v>
-      </c>
       <c r="C16" s="1" t="n">
         <v>15</v>
       </c>
-      <c r="G16" s="1" t="n">
+      <c r="F16" s="1" t="n">
         <v>0.1483</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B17" s="2" t="s">
         <v>13</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>14</v>
       </c>
       <c r="C17" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="G17" s="1" t="n">
+      <c r="F17" s="1" t="n">
         <v>0.1555</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B18" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B18" s="2" t="s">
-        <v>14</v>
-      </c>
       <c r="C18" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="G18" s="1" t="n">
+      <c r="F18" s="1" t="n">
         <v>0.1467</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B19" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B19" s="2" t="s">
-        <v>14</v>
-      </c>
       <c r="C19" s="1" t="n">
         <v>9</v>
       </c>
-      <c r="G19" s="1" t="n">
+      <c r="F19" s="1" t="n">
         <v>0.1483</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B20" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B20" s="2" t="s">
-        <v>14</v>
-      </c>
       <c r="C20" s="1" t="n">
         <v>12</v>
       </c>
-      <c r="G20" s="1" t="n">
+      <c r="F20" s="1" t="n">
         <v>0.1483</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B21" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B21" s="2" t="s">
-        <v>14</v>
-      </c>
       <c r="C21" s="1" t="n">
         <v>15</v>
       </c>
-      <c r="G21" s="1" t="n">
+      <c r="F21" s="1" t="n">
         <v>0.1483</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C22" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="G22" s="1" t="n">
+      <c r="F22" s="1" t="n">
         <v>0.145</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C23" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="G23" s="1" t="n">
+      <c r="F23" s="1" t="n">
         <v>0.145</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C24" s="1" t="n">
         <v>9</v>
       </c>
-      <c r="G24" s="1" t="n">
+      <c r="F24" s="1" t="n">
         <v>0.1467</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C25" s="1" t="n">
         <v>12</v>
       </c>
-      <c r="G25" s="1" t="n">
+      <c r="F25" s="1" t="n">
         <v>0.1467</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C26" s="1" t="n">
         <v>15</v>
       </c>
-      <c r="G26" s="1" t="n">
+      <c r="F26" s="1" t="n">
         <v>0.1467</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B27" s="2" t="s">
         <v>17</v>
-      </c>
-      <c r="B27" s="2" t="s">
-        <v>18</v>
       </c>
       <c r="C27" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="G27" s="1" t="n">
+      <c r="F27" s="1" t="n">
         <v>0.1531</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B28" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B28" s="2" t="s">
-        <v>18</v>
-      </c>
       <c r="C28" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="G28" s="1" t="n">
+      <c r="F28" s="1" t="n">
         <v>0.1531</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B29" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B29" s="2" t="s">
-        <v>18</v>
-      </c>
       <c r="C29" s="1" t="n">
         <v>9</v>
       </c>
-      <c r="G29" s="1" t="n">
+      <c r="F29" s="1" t="n">
         <v>0.1562</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B30" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B30" s="2" t="s">
-        <v>18</v>
-      </c>
       <c r="C30" s="1" t="n">
         <v>12</v>
       </c>
-      <c r="G30" s="1" t="n">
+      <c r="F30" s="1" t="n">
         <v>0.1562</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B31" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B31" s="2" t="s">
-        <v>18</v>
-      </c>
       <c r="C31" s="1" t="n">
         <v>15</v>
       </c>
-      <c r="G31" s="1" t="n">
+      <c r="F31" s="1" t="n">
         <v>0.1562</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B32" s="2" t="s">
         <v>19</v>
-      </c>
-      <c r="B32" s="2" t="s">
-        <v>20</v>
       </c>
       <c r="C32" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="G32" s="1" t="n">
+      <c r="F32" s="1" t="n">
         <v>0.1524</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B33" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B33" s="2" t="s">
-        <v>20</v>
-      </c>
       <c r="C33" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="G33" s="1" t="n">
+      <c r="F33" s="1" t="n">
         <v>0.1524</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B34" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B34" s="2" t="s">
-        <v>20</v>
-      </c>
       <c r="C34" s="1" t="n">
         <v>9</v>
       </c>
-      <c r="G34" s="1" t="n">
+      <c r="F34" s="1" t="n">
         <v>0.1555</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B35" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B35" s="2" t="s">
-        <v>20</v>
-      </c>
       <c r="C35" s="1" t="n">
         <v>12</v>
       </c>
-      <c r="G35" s="1" t="n">
+      <c r="F35" s="1" t="n">
         <v>0.1555</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B36" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B36" s="2" t="s">
-        <v>20</v>
-      </c>
       <c r="C36" s="1" t="n">
         <v>15</v>
       </c>
-      <c r="G36" s="1" t="n">
+      <c r="F36" s="1" t="n">
         <v>0.1555</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B37" s="2" t="s">
         <v>21</v>
-      </c>
-      <c r="B37" s="2" t="s">
-        <v>22</v>
       </c>
       <c r="C37" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="G37" s="1" t="n">
+      <c r="F37" s="1" t="n">
         <v>0.1546</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B38" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B38" s="2" t="s">
-        <v>22</v>
-      </c>
       <c r="C38" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="G38" s="1" t="n">
+      <c r="F38" s="1" t="n">
         <v>0.1546</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B39" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B39" s="2" t="s">
-        <v>22</v>
-      </c>
       <c r="C39" s="1" t="n">
         <v>9</v>
       </c>
-      <c r="G39" s="1" t="n">
+      <c r="F39" s="1" t="n">
         <v>0.1587</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B40" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B40" s="2" t="s">
-        <v>22</v>
-      </c>
       <c r="C40" s="1" t="n">
         <v>12</v>
       </c>
-      <c r="G40" s="1" t="n">
+      <c r="F40" s="1" t="n">
         <v>0.1587</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B41" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B41" s="2" t="s">
-        <v>22</v>
-      </c>
       <c r="C41" s="1" t="n">
         <v>15</v>
       </c>
-      <c r="G41" s="1" t="n">
+      <c r="F41" s="1" t="n">
         <v>0.1587</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B42" s="2" t="s">
         <v>23</v>
-      </c>
-      <c r="B42" s="2" t="s">
-        <v>24</v>
       </c>
       <c r="C42" s="1" t="n">
         <v>3</v>
@@ -1005,16 +994,16 @@
         <f aca="false">12*8.59</f>
         <v>103.08</v>
       </c>
-      <c r="G42" s="3" t="n">
+      <c r="F42" s="1" t="n">
         <v>0.15566</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B43" s="2" t="s">
         <v>23</v>
-      </c>
-      <c r="B43" s="2" t="s">
-        <v>24</v>
       </c>
       <c r="C43" s="1" t="n">
         <v>6</v>
@@ -1023,16 +1012,16 @@
         <f aca="false">12*10.66</f>
         <v>127.92</v>
       </c>
-      <c r="G43" s="3" t="n">
+      <c r="F43" s="1" t="n">
         <v>0.15566</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B44" s="2" t="s">
         <v>23</v>
-      </c>
-      <c r="B44" s="2" t="s">
-        <v>24</v>
       </c>
       <c r="C44" s="1" t="n">
         <v>9</v>
@@ -1041,16 +1030,16 @@
         <f aca="false">12*12.72</f>
         <v>152.64</v>
       </c>
-      <c r="G44" s="1" t="n">
+      <c r="F44" s="1" t="n">
         <v>0.15974</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B45" s="2" t="s">
         <v>23</v>
-      </c>
-      <c r="B45" s="2" t="s">
-        <v>24</v>
       </c>
       <c r="C45" s="1" t="n">
         <v>12</v>
@@ -1059,16 +1048,16 @@
         <f aca="false">12*14.79</f>
         <v>177.48</v>
       </c>
-      <c r="G45" s="1" t="n">
+      <c r="F45" s="1" t="n">
         <v>0.15974</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B46" s="2" t="s">
         <v>23</v>
-      </c>
-      <c r="B46" s="2" t="s">
-        <v>24</v>
       </c>
       <c r="C46" s="1" t="n">
         <v>15</v>
@@ -1077,86 +1066,86 @@
         <f aca="false">12*16.79</f>
         <v>201.48</v>
       </c>
-      <c r="G46" s="1" t="n">
+      <c r="F46" s="1" t="n">
         <v>0.15974</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B47" s="2" t="s">
         <v>25</v>
-      </c>
-      <c r="B47" s="2" t="s">
-        <v>26</v>
       </c>
       <c r="C47" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="G47" s="1" t="n">
+      <c r="F47" s="1" t="n">
         <v>0.1582</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B48" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B48" s="2" t="s">
-        <v>26</v>
-      </c>
       <c r="C48" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="G48" s="1" t="n">
+      <c r="F48" s="1" t="n">
         <v>0.1582</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B49" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B49" s="2" t="s">
-        <v>26</v>
-      </c>
       <c r="C49" s="1" t="n">
         <v>9</v>
       </c>
-      <c r="G49" s="1" t="n">
+      <c r="F49" s="1" t="n">
         <v>0.163</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B50" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B50" s="2" t="s">
-        <v>26</v>
-      </c>
       <c r="C50" s="1" t="n">
         <v>12</v>
       </c>
-      <c r="G50" s="1" t="n">
+      <c r="F50" s="1" t="n">
         <v>0.163</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B51" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B51" s="2" t="s">
-        <v>26</v>
-      </c>
       <c r="C51" s="1" t="n">
         <v>15</v>
       </c>
-      <c r="G51" s="1" t="n">
+      <c r="F51" s="1" t="n">
         <v>0.163</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B52" s="2" t="s">
         <v>27</v>
-      </c>
-      <c r="B52" s="2" t="s">
-        <v>28</v>
       </c>
       <c r="C52" s="1" t="n">
         <v>3</v>
@@ -1165,16 +1154,16 @@
         <f aca="false">12*8.75</f>
         <v>105</v>
       </c>
-      <c r="G52" s="1" t="n">
+      <c r="F52" s="1" t="n">
         <v>0.15581</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B53" s="2" t="s">
         <v>27</v>
-      </c>
-      <c r="B53" s="2" t="s">
-        <v>28</v>
       </c>
       <c r="C53" s="1" t="n">
         <v>6</v>
@@ -1183,16 +1172,16 @@
         <f aca="false">12*11.48</f>
         <v>137.76</v>
       </c>
-      <c r="G53" s="1" t="n">
+      <c r="F53" s="1" t="n">
         <v>0.15581</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B54" s="2" t="s">
         <v>27</v>
-      </c>
-      <c r="B54" s="2" t="s">
-        <v>28</v>
       </c>
       <c r="C54" s="1" t="n">
         <v>9</v>
@@ -1201,16 +1190,16 @@
         <f aca="false">12*14.28</f>
         <v>171.36</v>
       </c>
-      <c r="G54" s="1" t="n">
+      <c r="F54" s="1" t="n">
         <v>0.16049</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B55" s="2" t="s">
         <v>27</v>
-      </c>
-      <c r="B55" s="2" t="s">
-        <v>28</v>
       </c>
       <c r="C55" s="1" t="n">
         <v>12</v>
@@ -1219,16 +1208,16 @@
         <f aca="false">12*17.13</f>
         <v>205.56</v>
       </c>
-      <c r="G55" s="1" t="n">
+      <c r="F55" s="1" t="n">
         <v>0.16049</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B56" s="2" t="s">
         <v>27</v>
-      </c>
-      <c r="B56" s="2" t="s">
-        <v>28</v>
       </c>
       <c r="C56" s="1" t="n">
         <v>15</v>
@@ -1237,296 +1226,296 @@
         <f aca="false">12*19.81</f>
         <v>237.72</v>
       </c>
-      <c r="G56" s="1" t="n">
+      <c r="F56" s="1" t="n">
         <v>0.16049</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B57" s="2" t="s">
         <v>27</v>
-      </c>
-      <c r="B57" s="2" t="s">
-        <v>28</v>
       </c>
       <c r="C57" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="G57" s="1" t="n">
+      <c r="F57" s="1" t="n">
         <v>0.174</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B58" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="B58" s="2" t="s">
-        <v>30</v>
-      </c>
       <c r="C58" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="G58" s="1" t="n">
+      <c r="F58" s="1" t="n">
         <v>0.174</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B59" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="B59" s="2" t="s">
-        <v>30</v>
-      </c>
       <c r="C59" s="1" t="n">
         <v>9</v>
       </c>
-      <c r="G59" s="1" t="n">
+      <c r="F59" s="1" t="n">
         <v>0.174</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B60" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="B60" s="2" t="s">
-        <v>30</v>
-      </c>
       <c r="C60" s="1" t="n">
         <v>12</v>
       </c>
-      <c r="G60" s="1" t="n">
+      <c r="F60" s="1" t="n">
         <v>0.174</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B61" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="B61" s="2" t="s">
-        <v>30</v>
-      </c>
       <c r="C61" s="1" t="n">
         <v>15</v>
       </c>
-      <c r="G61" s="1" t="n">
+      <c r="F61" s="1" t="n">
         <v>0.174</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B62" s="2" t="s">
         <v>31</v>
-      </c>
-      <c r="B62" s="2" t="s">
-        <v>32</v>
       </c>
       <c r="C62" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="G62" s="1" t="n">
+      <c r="F62" s="1" t="n">
         <v>0.174</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B63" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B63" s="2" t="s">
-        <v>32</v>
-      </c>
       <c r="C63" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="G63" s="1" t="n">
+      <c r="F63" s="1" t="n">
         <v>0.174</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B64" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B64" s="2" t="s">
-        <v>32</v>
-      </c>
       <c r="C64" s="1" t="n">
         <v>9</v>
       </c>
-      <c r="G64" s="1" t="n">
+      <c r="F64" s="1" t="n">
         <v>0.174</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B65" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B65" s="2" t="s">
-        <v>32</v>
-      </c>
       <c r="C65" s="1" t="n">
         <v>12</v>
       </c>
-      <c r="G65" s="1" t="n">
+      <c r="F65" s="1" t="n">
         <v>0.174</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B66" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B66" s="2" t="s">
-        <v>32</v>
-      </c>
       <c r="C66" s="1" t="n">
         <v>15</v>
       </c>
-      <c r="G66" s="1" t="n">
+      <c r="F66" s="1" t="n">
         <v>0.174</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B67" s="2" t="s">
         <v>33</v>
-      </c>
-      <c r="B67" s="2" t="s">
-        <v>34</v>
       </c>
       <c r="C67" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="G67" s="1" t="n">
+      <c r="F67" s="1" t="n">
         <v>0.2062</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B68" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="B68" s="2" t="s">
-        <v>34</v>
-      </c>
       <c r="C68" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="G68" s="1" t="n">
+      <c r="F68" s="1" t="n">
         <v>0.2062</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B69" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="B69" s="2" t="s">
-        <v>34</v>
-      </c>
       <c r="C69" s="1" t="n">
         <v>9</v>
       </c>
-      <c r="G69" s="1" t="n">
+      <c r="F69" s="1" t="n">
         <v>0.2062</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B70" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="B70" s="2" t="s">
-        <v>34</v>
-      </c>
       <c r="C70" s="1" t="n">
         <v>12</v>
       </c>
-      <c r="G70" s="1" t="n">
+      <c r="F70" s="1" t="n">
         <v>0.2062</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B71" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="B71" s="2" t="s">
-        <v>34</v>
-      </c>
       <c r="C71" s="1" t="n">
         <v>15</v>
       </c>
-      <c r="G71" s="1" t="n">
+      <c r="F71" s="1" t="n">
         <v>0.2062</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B72" s="2" t="s">
         <v>35</v>
-      </c>
-      <c r="B72" s="2" t="s">
-        <v>36</v>
       </c>
       <c r="C72" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="G72" s="1" t="n">
+      <c r="F72" s="1" t="n">
         <v>0.2276</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B73" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="B73" s="2" t="s">
-        <v>36</v>
-      </c>
       <c r="C73" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="G73" s="1" t="n">
+      <c r="F73" s="1" t="n">
         <v>0.2276</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B74" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="B74" s="2" t="s">
-        <v>36</v>
-      </c>
       <c r="C74" s="1" t="n">
         <v>9</v>
       </c>
-      <c r="G74" s="1" t="n">
+      <c r="F74" s="1" t="n">
         <v>0.2276</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B75" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="B75" s="2" t="s">
-        <v>36</v>
-      </c>
       <c r="C75" s="1" t="n">
         <v>12</v>
       </c>
-      <c r="G75" s="1" t="n">
+      <c r="F75" s="1" t="n">
         <v>0.2276</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B76" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="B76" s="2" t="s">
-        <v>36</v>
-      </c>
       <c r="C76" s="1" t="n">
         <v>15</v>
       </c>
-      <c r="G76" s="1" t="n">
+      <c r="F76" s="1" t="n">
         <v>0.2276</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B77" s="2" t="s">
         <v>37</v>
-      </c>
-      <c r="B77" s="2" t="s">
-        <v>38</v>
       </c>
       <c r="C77" s="1" t="n">
         <v>3</v>
@@ -1535,16 +1524,16 @@
         <f aca="false">12*9.69</f>
         <v>116.28</v>
       </c>
-      <c r="G77" s="1" t="n">
+      <c r="F77" s="1" t="n">
         <v>0.25164</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B78" s="2" t="s">
         <v>37</v>
-      </c>
-      <c r="B78" s="2" t="s">
-        <v>38</v>
       </c>
       <c r="C78" s="1" t="n">
         <v>6</v>
@@ -1553,16 +1542,16 @@
         <f aca="false">12*12.71</f>
         <v>152.52</v>
       </c>
-      <c r="G78" s="1" t="n">
+      <c r="F78" s="1" t="n">
         <v>0.25164</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B79" s="2" t="s">
         <v>37</v>
-      </c>
-      <c r="B79" s="2" t="s">
-        <v>38</v>
       </c>
       <c r="C79" s="1" t="n">
         <v>9</v>
@@ -1571,16 +1560,16 @@
         <f aca="false">12*15.96</f>
         <v>191.52</v>
       </c>
-      <c r="G79" s="1" t="n">
+      <c r="F79" s="1" t="n">
         <v>0.25164</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B80" s="2" t="s">
         <v>37</v>
-      </c>
-      <c r="B80" s="2" t="s">
-        <v>38</v>
       </c>
       <c r="C80" s="1" t="n">
         <v>12</v>
@@ -1589,16 +1578,16 @@
         <f aca="false">12*19.27</f>
         <v>231.24</v>
       </c>
-      <c r="G80" s="1" t="n">
+      <c r="F80" s="1" t="n">
         <v>0.25164</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B81" s="2" t="s">
         <v>37</v>
-      </c>
-      <c r="B81" s="2" t="s">
-        <v>38</v>
       </c>
       <c r="C81" s="1" t="n">
         <v>15</v>
@@ -1607,16 +1596,16 @@
         <f aca="false">12*22.35</f>
         <v>268.2</v>
       </c>
-      <c r="G81" s="1" t="n">
+      <c r="F81" s="1" t="n">
         <v>0.25164</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B82" s="2" t="s">
         <v>39</v>
-      </c>
-      <c r="B82" s="2" t="s">
-        <v>40</v>
       </c>
       <c r="C82" s="1" t="n">
         <v>3</v>
@@ -1625,16 +1614,16 @@
         <f aca="false">12*10.48</f>
         <v>125.76</v>
       </c>
-      <c r="G82" s="1" t="n">
+      <c r="F82" s="1" t="n">
         <v>0.2016</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B83" s="2" t="s">
         <v>39</v>
-      </c>
-      <c r="B83" s="2" t="s">
-        <v>40</v>
       </c>
       <c r="C83" s="1" t="n">
         <v>6</v>
@@ -1643,16 +1632,16 @@
         <f aca="false">12*13.86</f>
         <v>166.32</v>
       </c>
-      <c r="G83" s="1" t="n">
+      <c r="F83" s="1" t="n">
         <v>0.2016</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B84" s="2" t="s">
         <v>41</v>
-      </c>
-      <c r="B84" s="2" t="s">
-        <v>42</v>
       </c>
       <c r="C84" s="1" t="n">
         <v>3</v>
@@ -1661,16 +1650,16 @@
         <f aca="false">12*11.79</f>
         <v>141.48</v>
       </c>
-      <c r="G84" s="1" t="n">
+      <c r="F84" s="1" t="n">
         <v>0.19522</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B85" s="2" t="s">
         <v>41</v>
-      </c>
-      <c r="B85" s="2" t="s">
-        <v>42</v>
       </c>
       <c r="C85" s="1" t="n">
         <v>6</v>
@@ -1679,16 +1668,16 @@
         <f aca="false">12*15.59</f>
         <v>187.08</v>
       </c>
-      <c r="G85" s="1" t="n">
+      <c r="F85" s="1" t="n">
         <v>0.19522</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B86" s="2" t="s">
         <v>41</v>
-      </c>
-      <c r="B86" s="2" t="s">
-        <v>42</v>
       </c>
       <c r="C86" s="1" t="n">
         <v>9</v>
@@ -1697,16 +1686,16 @@
         <f aca="false">12*19.58</f>
         <v>234.96</v>
       </c>
-      <c r="G86" s="1" t="n">
+      <c r="F86" s="1" t="n">
         <v>0.19522</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B87" s="2" t="s">
         <v>41</v>
-      </c>
-      <c r="B87" s="2" t="s">
-        <v>42</v>
       </c>
       <c r="C87" s="1" t="n">
         <v>12</v>
@@ -1715,16 +1704,16 @@
         <f aca="false">12*23.58</f>
         <v>282.96</v>
       </c>
-      <c r="G87" s="1" t="n">
+      <c r="F87" s="1" t="n">
         <v>0.19522</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B88" s="2" t="s">
         <v>41</v>
-      </c>
-      <c r="B88" s="2" t="s">
-        <v>42</v>
       </c>
       <c r="C88" s="1" t="n">
         <v>15</v>
@@ -1733,16 +1722,16 @@
         <f aca="false">12*27.38</f>
         <v>328.56</v>
       </c>
-      <c r="G88" s="1" t="n">
+      <c r="F88" s="1" t="n">
         <v>0.19522</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B89" s="2" t="s">
         <v>41</v>
-      </c>
-      <c r="B89" s="2" t="s">
-        <v>42</v>
       </c>
       <c r="C89" s="1" t="n">
         <v>18</v>
@@ -1751,16 +1740,16 @@
         <f aca="false">12*31.14</f>
         <v>373.68</v>
       </c>
-      <c r="G89" s="1" t="n">
+      <c r="F89" s="1" t="n">
         <v>0.19522</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B90" s="2" t="s">
         <v>41</v>
-      </c>
-      <c r="B90" s="2" t="s">
-        <v>42</v>
       </c>
       <c r="C90" s="1" t="n">
         <v>24</v>
@@ -1769,16 +1758,16 @@
         <f aca="false">12*39.29</f>
         <v>471.48</v>
       </c>
-      <c r="G90" s="1" t="n">
+      <c r="F90" s="1" t="n">
         <v>0.19522</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B91" s="2" t="s">
         <v>41</v>
-      </c>
-      <c r="B91" s="2" t="s">
-        <v>42</v>
       </c>
       <c r="C91" s="1" t="n">
         <v>30</v>
@@ -1787,16 +1776,16 @@
         <f aca="false">12*47.07</f>
         <v>564.84</v>
       </c>
-      <c r="G91" s="1" t="n">
+      <c r="F91" s="1" t="n">
         <v>0.19522</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B92" s="2" t="s">
         <v>41</v>
-      </c>
-      <c r="B92" s="2" t="s">
-        <v>42</v>
       </c>
       <c r="C92" s="1" t="n">
         <v>36</v>
@@ -1805,89 +1794,179 @@
         <f aca="false">12*55.05</f>
         <v>660.6</v>
       </c>
-      <c r="G92" s="1" t="n">
+      <c r="F92" s="1" t="n">
         <v>0.19522</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A93" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B93" s="2"/>
       <c r="C93" s="1" t="n">
         <v>3</v>
       </c>
+      <c r="D93" s="1" t="n">
+        <v>12.07</v>
+      </c>
+      <c r="E93" s="1" t="n">
+        <f aca="false">IF(D93="","",12*D93)</f>
+        <v>144.84</v>
+      </c>
+      <c r="F93" s="1" t="n">
+        <v>0.19398</v>
+      </c>
     </row>
     <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A94" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B94" s="2"/>
       <c r="C94" s="1" t="n">
         <v>6</v>
       </c>
+      <c r="D94" s="1" t="n">
+        <v>15.74</v>
+      </c>
+      <c r="E94" s="1" t="n">
+        <f aca="false">IF(D94="","",12*D94)</f>
+        <v>188.88</v>
+      </c>
+      <c r="F94" s="1" t="n">
+        <v>0.19398</v>
+      </c>
     </row>
     <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A95" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B95" s="2"/>
       <c r="C95" s="1" t="n">
         <v>9</v>
       </c>
+      <c r="D95" s="1" t="n">
+        <v>19.69</v>
+      </c>
+      <c r="E95" s="1" t="n">
+        <f aca="false">IF(D95="","",12*D95)</f>
+        <v>236.28</v>
+      </c>
+      <c r="F95" s="1" t="n">
+        <v>0.19266</v>
+      </c>
     </row>
     <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A96" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B96" s="2"/>
       <c r="C96" s="1" t="n">
         <v>12</v>
       </c>
+      <c r="D96" s="1" t="n">
+        <v>23.49</v>
+      </c>
+      <c r="E96" s="1" t="n">
+        <f aca="false">IF(D96="","",12*D96)</f>
+        <v>281.88</v>
+      </c>
+      <c r="F96" s="1" t="n">
+        <v>0.19266</v>
+      </c>
     </row>
     <row r="97" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A97" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B97" s="2"/>
       <c r="C97" s="1" t="n">
         <v>15</v>
       </c>
+      <c r="D97" s="1" t="n">
+        <v>27.06</v>
+      </c>
+      <c r="E97" s="1" t="n">
+        <f aca="false">IF(D97="","",12*D97)</f>
+        <v>324.72</v>
+      </c>
+      <c r="F97" s="1" t="n">
+        <v>0.19266</v>
+      </c>
     </row>
     <row r="98" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A98" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B98" s="2"/>
       <c r="C98" s="1" t="n">
         <v>18</v>
       </c>
+      <c r="D98" s="1" t="n">
+        <v>30.75</v>
+      </c>
+      <c r="E98" s="1" t="n">
+        <f aca="false">IF(D98="","",12*D98)</f>
+        <v>369</v>
+      </c>
+      <c r="F98" s="1" t="n">
+        <v>0.19266</v>
+      </c>
     </row>
     <row r="99" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A99" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B99" s="2"/>
       <c r="C99" s="1" t="n">
         <v>24</v>
       </c>
+      <c r="D99" s="1" t="n">
+        <v>38.59</v>
+      </c>
+      <c r="E99" s="1" t="n">
+        <f aca="false">IF(D99="","",12*D99)</f>
+        <v>463.08</v>
+      </c>
+      <c r="F99" s="1" t="n">
+        <v>0.19266</v>
+      </c>
     </row>
     <row r="100" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A100" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B100" s="2"/>
       <c r="C100" s="1" t="n">
         <v>30</v>
       </c>
+      <c r="D100" s="1" t="n">
+        <v>45.8</v>
+      </c>
+      <c r="E100" s="1" t="n">
+        <f aca="false">IF(D100="","",12*D100)</f>
+        <v>549.6</v>
+      </c>
+      <c r="F100" s="1" t="n">
+        <v>0.19266</v>
+      </c>
     </row>
     <row r="101" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A101" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B101" s="2"/>
       <c r="C101" s="1" t="n">
         <v>36</v>
+      </c>
+      <c r="D101" s="1" t="n">
+        <v>53.06</v>
+      </c>
+      <c r="E101" s="1" t="n">
+        <f aca="false">IF(D101="","",12*D101)</f>
+        <v>636.72</v>
+      </c>
+      <c r="F101" s="1" t="n">
+        <v>0.19266</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update Electricité de Strasbourg prices of 2026-02-01 (#12)
</commit_message>
<xml_diff>
--- a/contracts/electricite-de-strasbourg/tarif-bleu-base/Option_Base.xlsx
+++ b/contracts/electricite-de-strasbourg/tarif-bleu-base/Option_Base.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="43">
   <si>
     <t xml:space="preserve">DATE_DEBUT</t>
   </si>
@@ -31,13 +31,10 @@
     <t xml:space="preserve">P_SOUSCRITE</t>
   </si>
   <si>
-    <t xml:space="preserve">PART_FIXE_HT</t>
+    <t xml:space="preserve">PART_FIXE_TTC_MOIS</t>
   </si>
   <si>
     <t xml:space="preserve">PART_FIXE_TTC</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PART_VARIABLE_HT</t>
   </si>
   <si>
     <t xml:space="preserve">PART_VARIABLE_TTC</t>
@@ -227,7 +224,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -237,10 +234,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -367,14 +360,14 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G101"/>
+  <dimension ref="A1:F101"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B65" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B77" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="A65" activeCellId="0" sqref="A65"/>
-      <selection pane="bottomRight" activeCell="B77" activeCellId="0" sqref="B77"/>
+      <selection pane="bottomLeft" activeCell="A77" activeCellId="0" sqref="A77"/>
+      <selection pane="bottomRight" activeCell="F94" activeCellId="0" sqref="F94"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -384,8 +377,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="14.03"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="14.62"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="13.41"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="19.35"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="20.45"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="20.45"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -407,16 +399,13 @@
       <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>6</v>
-      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>7</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>8</v>
       </c>
       <c r="C2" s="1" t="n">
         <v>3</v>
@@ -425,16 +414,16 @@
         <f aca="false">12*4.54</f>
         <v>54.48</v>
       </c>
-      <c r="G2" s="1" t="n">
+      <c r="F2" s="1" t="n">
         <v>0.1503</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>7</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>8</v>
       </c>
       <c r="C3" s="1" t="n">
         <v>6</v>
@@ -443,16 +432,16 @@
         <f aca="false">12*7.37</f>
         <v>88.44</v>
       </c>
-      <c r="G3" s="1" t="n">
+      <c r="F3" s="1" t="n">
         <v>0.1503</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>7</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>8</v>
       </c>
       <c r="C4" s="1" t="n">
         <v>9</v>
@@ -461,16 +450,16 @@
         <f aca="false">12*9.77</f>
         <v>117.24</v>
       </c>
-      <c r="G4" s="1" t="n">
+      <c r="F4" s="1" t="n">
         <v>0.1503</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>7</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>8</v>
       </c>
       <c r="C5" s="1" t="n">
         <v>12</v>
@@ -479,16 +468,16 @@
         <f aca="false">12*15.01</f>
         <v>180.12</v>
       </c>
-      <c r="G5" s="1" t="n">
+      <c r="F5" s="1" t="n">
         <v>0.1503</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="2" t="s">
         <v>7</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>8</v>
       </c>
       <c r="C6" s="1" t="n">
         <v>15</v>
@@ -497,506 +486,506 @@
         <f aca="false">12*17.21</f>
         <v>206.52</v>
       </c>
-      <c r="G6" s="1" t="n">
+      <c r="F6" s="1" t="n">
         <v>0.1503</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C7" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="G7" s="1" t="n">
+      <c r="F7" s="1" t="n">
         <v>0.1503</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C8" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="G8" s="1" t="n">
+      <c r="F8" s="1" t="n">
         <v>0.1503</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C9" s="1" t="n">
         <v>9</v>
       </c>
-      <c r="G9" s="1" t="n">
+      <c r="F9" s="1" t="n">
         <v>0.1503</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C10" s="1" t="n">
         <v>12</v>
       </c>
-      <c r="G10" s="1" t="n">
+      <c r="F10" s="1" t="n">
         <v>0.1503</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C11" s="1" t="n">
         <v>15</v>
       </c>
-      <c r="G11" s="1" t="n">
+      <c r="F11" s="1" t="n">
         <v>0.1503</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B12" s="2" t="s">
         <v>11</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>12</v>
       </c>
       <c r="C12" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="G12" s="1" t="n">
+      <c r="F12" s="1" t="n">
         <v>0.1546</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B13" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B13" s="2" t="s">
-        <v>12</v>
-      </c>
       <c r="C13" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="G13" s="1" t="n">
+      <c r="F13" s="1" t="n">
         <v>0.1466</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B14" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B14" s="2" t="s">
-        <v>12</v>
-      </c>
       <c r="C14" s="1" t="n">
         <v>9</v>
       </c>
-      <c r="G14" s="1" t="n">
+      <c r="F14" s="1" t="n">
         <v>0.1483</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B15" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B15" s="2" t="s">
-        <v>12</v>
-      </c>
       <c r="C15" s="1" t="n">
         <v>12</v>
       </c>
-      <c r="G15" s="1" t="n">
+      <c r="F15" s="1" t="n">
         <v>0.1483</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B16" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B16" s="2" t="s">
-        <v>12</v>
-      </c>
       <c r="C16" s="1" t="n">
         <v>15</v>
       </c>
-      <c r="G16" s="1" t="n">
+      <c r="F16" s="1" t="n">
         <v>0.1483</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B17" s="2" t="s">
         <v>13</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>14</v>
       </c>
       <c r="C17" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="G17" s="1" t="n">
+      <c r="F17" s="1" t="n">
         <v>0.1555</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B18" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B18" s="2" t="s">
-        <v>14</v>
-      </c>
       <c r="C18" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="G18" s="1" t="n">
+      <c r="F18" s="1" t="n">
         <v>0.1467</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B19" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B19" s="2" t="s">
-        <v>14</v>
-      </c>
       <c r="C19" s="1" t="n">
         <v>9</v>
       </c>
-      <c r="G19" s="1" t="n">
+      <c r="F19" s="1" t="n">
         <v>0.1483</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B20" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B20" s="2" t="s">
-        <v>14</v>
-      </c>
       <c r="C20" s="1" t="n">
         <v>12</v>
       </c>
-      <c r="G20" s="1" t="n">
+      <c r="F20" s="1" t="n">
         <v>0.1483</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B21" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B21" s="2" t="s">
-        <v>14</v>
-      </c>
       <c r="C21" s="1" t="n">
         <v>15</v>
       </c>
-      <c r="G21" s="1" t="n">
+      <c r="F21" s="1" t="n">
         <v>0.1483</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C22" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="G22" s="1" t="n">
+      <c r="F22" s="1" t="n">
         <v>0.145</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C23" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="G23" s="1" t="n">
+      <c r="F23" s="1" t="n">
         <v>0.145</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C24" s="1" t="n">
         <v>9</v>
       </c>
-      <c r="G24" s="1" t="n">
+      <c r="F24" s="1" t="n">
         <v>0.1467</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C25" s="1" t="n">
         <v>12</v>
       </c>
-      <c r="G25" s="1" t="n">
+      <c r="F25" s="1" t="n">
         <v>0.1467</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C26" s="1" t="n">
         <v>15</v>
       </c>
-      <c r="G26" s="1" t="n">
+      <c r="F26" s="1" t="n">
         <v>0.1467</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B27" s="2" t="s">
         <v>17</v>
-      </c>
-      <c r="B27" s="2" t="s">
-        <v>18</v>
       </c>
       <c r="C27" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="G27" s="1" t="n">
+      <c r="F27" s="1" t="n">
         <v>0.1531</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B28" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B28" s="2" t="s">
-        <v>18</v>
-      </c>
       <c r="C28" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="G28" s="1" t="n">
+      <c r="F28" s="1" t="n">
         <v>0.1531</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B29" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B29" s="2" t="s">
-        <v>18</v>
-      </c>
       <c r="C29" s="1" t="n">
         <v>9</v>
       </c>
-      <c r="G29" s="1" t="n">
+      <c r="F29" s="1" t="n">
         <v>0.1562</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B30" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B30" s="2" t="s">
-        <v>18</v>
-      </c>
       <c r="C30" s="1" t="n">
         <v>12</v>
       </c>
-      <c r="G30" s="1" t="n">
+      <c r="F30" s="1" t="n">
         <v>0.1562</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B31" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B31" s="2" t="s">
-        <v>18</v>
-      </c>
       <c r="C31" s="1" t="n">
         <v>15</v>
       </c>
-      <c r="G31" s="1" t="n">
+      <c r="F31" s="1" t="n">
         <v>0.1562</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B32" s="2" t="s">
         <v>19</v>
-      </c>
-      <c r="B32" s="2" t="s">
-        <v>20</v>
       </c>
       <c r="C32" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="G32" s="1" t="n">
+      <c r="F32" s="1" t="n">
         <v>0.1524</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B33" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B33" s="2" t="s">
-        <v>20</v>
-      </c>
       <c r="C33" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="G33" s="1" t="n">
+      <c r="F33" s="1" t="n">
         <v>0.1524</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B34" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B34" s="2" t="s">
-        <v>20</v>
-      </c>
       <c r="C34" s="1" t="n">
         <v>9</v>
       </c>
-      <c r="G34" s="1" t="n">
+      <c r="F34" s="1" t="n">
         <v>0.1555</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B35" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B35" s="2" t="s">
-        <v>20</v>
-      </c>
       <c r="C35" s="1" t="n">
         <v>12</v>
       </c>
-      <c r="G35" s="1" t="n">
+      <c r="F35" s="1" t="n">
         <v>0.1555</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B36" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B36" s="2" t="s">
-        <v>20</v>
-      </c>
       <c r="C36" s="1" t="n">
         <v>15</v>
       </c>
-      <c r="G36" s="1" t="n">
+      <c r="F36" s="1" t="n">
         <v>0.1555</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B37" s="2" t="s">
         <v>21</v>
-      </c>
-      <c r="B37" s="2" t="s">
-        <v>22</v>
       </c>
       <c r="C37" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="G37" s="1" t="n">
+      <c r="F37" s="1" t="n">
         <v>0.1546</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B38" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B38" s="2" t="s">
-        <v>22</v>
-      </c>
       <c r="C38" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="G38" s="1" t="n">
+      <c r="F38" s="1" t="n">
         <v>0.1546</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B39" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B39" s="2" t="s">
-        <v>22</v>
-      </c>
       <c r="C39" s="1" t="n">
         <v>9</v>
       </c>
-      <c r="G39" s="1" t="n">
+      <c r="F39" s="1" t="n">
         <v>0.1587</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B40" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B40" s="2" t="s">
-        <v>22</v>
-      </c>
       <c r="C40" s="1" t="n">
         <v>12</v>
       </c>
-      <c r="G40" s="1" t="n">
+      <c r="F40" s="1" t="n">
         <v>0.1587</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B41" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B41" s="2" t="s">
-        <v>22</v>
-      </c>
       <c r="C41" s="1" t="n">
         <v>15</v>
       </c>
-      <c r="G41" s="1" t="n">
+      <c r="F41" s="1" t="n">
         <v>0.1587</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B42" s="2" t="s">
         <v>23</v>
-      </c>
-      <c r="B42" s="2" t="s">
-        <v>24</v>
       </c>
       <c r="C42" s="1" t="n">
         <v>3</v>
@@ -1005,16 +994,16 @@
         <f aca="false">12*8.59</f>
         <v>103.08</v>
       </c>
-      <c r="G42" s="3" t="n">
+      <c r="F42" s="1" t="n">
         <v>0.15566</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B43" s="2" t="s">
         <v>23</v>
-      </c>
-      <c r="B43" s="2" t="s">
-        <v>24</v>
       </c>
       <c r="C43" s="1" t="n">
         <v>6</v>
@@ -1023,16 +1012,16 @@
         <f aca="false">12*10.66</f>
         <v>127.92</v>
       </c>
-      <c r="G43" s="3" t="n">
+      <c r="F43" s="1" t="n">
         <v>0.15566</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B44" s="2" t="s">
         <v>23</v>
-      </c>
-      <c r="B44" s="2" t="s">
-        <v>24</v>
       </c>
       <c r="C44" s="1" t="n">
         <v>9</v>
@@ -1041,16 +1030,16 @@
         <f aca="false">12*12.72</f>
         <v>152.64</v>
       </c>
-      <c r="G44" s="1" t="n">
+      <c r="F44" s="1" t="n">
         <v>0.15974</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B45" s="2" t="s">
         <v>23</v>
-      </c>
-      <c r="B45" s="2" t="s">
-        <v>24</v>
       </c>
       <c r="C45" s="1" t="n">
         <v>12</v>
@@ -1059,16 +1048,16 @@
         <f aca="false">12*14.79</f>
         <v>177.48</v>
       </c>
-      <c r="G45" s="1" t="n">
+      <c r="F45" s="1" t="n">
         <v>0.15974</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B46" s="2" t="s">
         <v>23</v>
-      </c>
-      <c r="B46" s="2" t="s">
-        <v>24</v>
       </c>
       <c r="C46" s="1" t="n">
         <v>15</v>
@@ -1077,86 +1066,86 @@
         <f aca="false">12*16.79</f>
         <v>201.48</v>
       </c>
-      <c r="G46" s="1" t="n">
+      <c r="F46" s="1" t="n">
         <v>0.15974</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B47" s="2" t="s">
         <v>25</v>
-      </c>
-      <c r="B47" s="2" t="s">
-        <v>26</v>
       </c>
       <c r="C47" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="G47" s="1" t="n">
+      <c r="F47" s="1" t="n">
         <v>0.1582</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B48" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B48" s="2" t="s">
-        <v>26</v>
-      </c>
       <c r="C48" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="G48" s="1" t="n">
+      <c r="F48" s="1" t="n">
         <v>0.1582</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B49" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B49" s="2" t="s">
-        <v>26</v>
-      </c>
       <c r="C49" s="1" t="n">
         <v>9</v>
       </c>
-      <c r="G49" s="1" t="n">
+      <c r="F49" s="1" t="n">
         <v>0.163</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B50" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B50" s="2" t="s">
-        <v>26</v>
-      </c>
       <c r="C50" s="1" t="n">
         <v>12</v>
       </c>
-      <c r="G50" s="1" t="n">
+      <c r="F50" s="1" t="n">
         <v>0.163</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B51" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B51" s="2" t="s">
-        <v>26</v>
-      </c>
       <c r="C51" s="1" t="n">
         <v>15</v>
       </c>
-      <c r="G51" s="1" t="n">
+      <c r="F51" s="1" t="n">
         <v>0.163</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B52" s="2" t="s">
         <v>27</v>
-      </c>
-      <c r="B52" s="2" t="s">
-        <v>28</v>
       </c>
       <c r="C52" s="1" t="n">
         <v>3</v>
@@ -1165,16 +1154,16 @@
         <f aca="false">12*8.75</f>
         <v>105</v>
       </c>
-      <c r="G52" s="1" t="n">
+      <c r="F52" s="1" t="n">
         <v>0.15581</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B53" s="2" t="s">
         <v>27</v>
-      </c>
-      <c r="B53" s="2" t="s">
-        <v>28</v>
       </c>
       <c r="C53" s="1" t="n">
         <v>6</v>
@@ -1183,16 +1172,16 @@
         <f aca="false">12*11.48</f>
         <v>137.76</v>
       </c>
-      <c r="G53" s="1" t="n">
+      <c r="F53" s="1" t="n">
         <v>0.15581</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B54" s="2" t="s">
         <v>27</v>
-      </c>
-      <c r="B54" s="2" t="s">
-        <v>28</v>
       </c>
       <c r="C54" s="1" t="n">
         <v>9</v>
@@ -1201,16 +1190,16 @@
         <f aca="false">12*14.28</f>
         <v>171.36</v>
       </c>
-      <c r="G54" s="1" t="n">
+      <c r="F54" s="1" t="n">
         <v>0.16049</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B55" s="2" t="s">
         <v>27</v>
-      </c>
-      <c r="B55" s="2" t="s">
-        <v>28</v>
       </c>
       <c r="C55" s="1" t="n">
         <v>12</v>
@@ -1219,16 +1208,16 @@
         <f aca="false">12*17.13</f>
         <v>205.56</v>
       </c>
-      <c r="G55" s="1" t="n">
+      <c r="F55" s="1" t="n">
         <v>0.16049</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B56" s="2" t="s">
         <v>27</v>
-      </c>
-      <c r="B56" s="2" t="s">
-        <v>28</v>
       </c>
       <c r="C56" s="1" t="n">
         <v>15</v>
@@ -1237,296 +1226,296 @@
         <f aca="false">12*19.81</f>
         <v>237.72</v>
       </c>
-      <c r="G56" s="1" t="n">
+      <c r="F56" s="1" t="n">
         <v>0.16049</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B57" s="2" t="s">
         <v>27</v>
-      </c>
-      <c r="B57" s="2" t="s">
-        <v>28</v>
       </c>
       <c r="C57" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="G57" s="1" t="n">
+      <c r="F57" s="1" t="n">
         <v>0.174</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B58" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="B58" s="2" t="s">
-        <v>30</v>
-      </c>
       <c r="C58" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="G58" s="1" t="n">
+      <c r="F58" s="1" t="n">
         <v>0.174</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B59" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="B59" s="2" t="s">
-        <v>30</v>
-      </c>
       <c r="C59" s="1" t="n">
         <v>9</v>
       </c>
-      <c r="G59" s="1" t="n">
+      <c r="F59" s="1" t="n">
         <v>0.174</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B60" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="B60" s="2" t="s">
-        <v>30</v>
-      </c>
       <c r="C60" s="1" t="n">
         <v>12</v>
       </c>
-      <c r="G60" s="1" t="n">
+      <c r="F60" s="1" t="n">
         <v>0.174</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B61" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="B61" s="2" t="s">
-        <v>30</v>
-      </c>
       <c r="C61" s="1" t="n">
         <v>15</v>
       </c>
-      <c r="G61" s="1" t="n">
+      <c r="F61" s="1" t="n">
         <v>0.174</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B62" s="2" t="s">
         <v>31</v>
-      </c>
-      <c r="B62" s="2" t="s">
-        <v>32</v>
       </c>
       <c r="C62" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="G62" s="1" t="n">
+      <c r="F62" s="1" t="n">
         <v>0.174</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B63" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B63" s="2" t="s">
-        <v>32</v>
-      </c>
       <c r="C63" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="G63" s="1" t="n">
+      <c r="F63" s="1" t="n">
         <v>0.174</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B64" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B64" s="2" t="s">
-        <v>32</v>
-      </c>
       <c r="C64" s="1" t="n">
         <v>9</v>
       </c>
-      <c r="G64" s="1" t="n">
+      <c r="F64" s="1" t="n">
         <v>0.174</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B65" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B65" s="2" t="s">
-        <v>32</v>
-      </c>
       <c r="C65" s="1" t="n">
         <v>12</v>
       </c>
-      <c r="G65" s="1" t="n">
+      <c r="F65" s="1" t="n">
         <v>0.174</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B66" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B66" s="2" t="s">
-        <v>32</v>
-      </c>
       <c r="C66" s="1" t="n">
         <v>15</v>
       </c>
-      <c r="G66" s="1" t="n">
+      <c r="F66" s="1" t="n">
         <v>0.174</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B67" s="2" t="s">
         <v>33</v>
-      </c>
-      <c r="B67" s="2" t="s">
-        <v>34</v>
       </c>
       <c r="C67" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="G67" s="1" t="n">
+      <c r="F67" s="1" t="n">
         <v>0.2062</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B68" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="B68" s="2" t="s">
-        <v>34</v>
-      </c>
       <c r="C68" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="G68" s="1" t="n">
+      <c r="F68" s="1" t="n">
         <v>0.2062</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B69" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="B69" s="2" t="s">
-        <v>34</v>
-      </c>
       <c r="C69" s="1" t="n">
         <v>9</v>
       </c>
-      <c r="G69" s="1" t="n">
+      <c r="F69" s="1" t="n">
         <v>0.2062</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B70" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="B70" s="2" t="s">
-        <v>34</v>
-      </c>
       <c r="C70" s="1" t="n">
         <v>12</v>
       </c>
-      <c r="G70" s="1" t="n">
+      <c r="F70" s="1" t="n">
         <v>0.2062</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B71" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="B71" s="2" t="s">
-        <v>34</v>
-      </c>
       <c r="C71" s="1" t="n">
         <v>15</v>
       </c>
-      <c r="G71" s="1" t="n">
+      <c r="F71" s="1" t="n">
         <v>0.2062</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B72" s="2" t="s">
         <v>35</v>
-      </c>
-      <c r="B72" s="2" t="s">
-        <v>36</v>
       </c>
       <c r="C72" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="G72" s="1" t="n">
+      <c r="F72" s="1" t="n">
         <v>0.2276</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B73" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="B73" s="2" t="s">
-        <v>36</v>
-      </c>
       <c r="C73" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="G73" s="1" t="n">
+      <c r="F73" s="1" t="n">
         <v>0.2276</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B74" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="B74" s="2" t="s">
-        <v>36</v>
-      </c>
       <c r="C74" s="1" t="n">
         <v>9</v>
       </c>
-      <c r="G74" s="1" t="n">
+      <c r="F74" s="1" t="n">
         <v>0.2276</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B75" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="B75" s="2" t="s">
-        <v>36</v>
-      </c>
       <c r="C75" s="1" t="n">
         <v>12</v>
       </c>
-      <c r="G75" s="1" t="n">
+      <c r="F75" s="1" t="n">
         <v>0.2276</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B76" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="B76" s="2" t="s">
-        <v>36</v>
-      </c>
       <c r="C76" s="1" t="n">
         <v>15</v>
       </c>
-      <c r="G76" s="1" t="n">
+      <c r="F76" s="1" t="n">
         <v>0.2276</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B77" s="2" t="s">
         <v>37</v>
-      </c>
-      <c r="B77" s="2" t="s">
-        <v>38</v>
       </c>
       <c r="C77" s="1" t="n">
         <v>3</v>
@@ -1535,16 +1524,16 @@
         <f aca="false">12*9.69</f>
         <v>116.28</v>
       </c>
-      <c r="G77" s="1" t="n">
+      <c r="F77" s="1" t="n">
         <v>0.25164</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B78" s="2" t="s">
         <v>37</v>
-      </c>
-      <c r="B78" s="2" t="s">
-        <v>38</v>
       </c>
       <c r="C78" s="1" t="n">
         <v>6</v>
@@ -1553,16 +1542,16 @@
         <f aca="false">12*12.71</f>
         <v>152.52</v>
       </c>
-      <c r="G78" s="1" t="n">
+      <c r="F78" s="1" t="n">
         <v>0.25164</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B79" s="2" t="s">
         <v>37</v>
-      </c>
-      <c r="B79" s="2" t="s">
-        <v>38</v>
       </c>
       <c r="C79" s="1" t="n">
         <v>9</v>
@@ -1571,16 +1560,16 @@
         <f aca="false">12*15.96</f>
         <v>191.52</v>
       </c>
-      <c r="G79" s="1" t="n">
+      <c r="F79" s="1" t="n">
         <v>0.25164</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B80" s="2" t="s">
         <v>37</v>
-      </c>
-      <c r="B80" s="2" t="s">
-        <v>38</v>
       </c>
       <c r="C80" s="1" t="n">
         <v>12</v>
@@ -1589,16 +1578,16 @@
         <f aca="false">12*19.27</f>
         <v>231.24</v>
       </c>
-      <c r="G80" s="1" t="n">
+      <c r="F80" s="1" t="n">
         <v>0.25164</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B81" s="2" t="s">
         <v>37</v>
-      </c>
-      <c r="B81" s="2" t="s">
-        <v>38</v>
       </c>
       <c r="C81" s="1" t="n">
         <v>15</v>
@@ -1607,16 +1596,16 @@
         <f aca="false">12*22.35</f>
         <v>268.2</v>
       </c>
-      <c r="G81" s="1" t="n">
+      <c r="F81" s="1" t="n">
         <v>0.25164</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B82" s="2" t="s">
         <v>39</v>
-      </c>
-      <c r="B82" s="2" t="s">
-        <v>40</v>
       </c>
       <c r="C82" s="1" t="n">
         <v>3</v>
@@ -1625,16 +1614,16 @@
         <f aca="false">12*10.48</f>
         <v>125.76</v>
       </c>
-      <c r="G82" s="1" t="n">
+      <c r="F82" s="1" t="n">
         <v>0.2016</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B83" s="2" t="s">
         <v>39</v>
-      </c>
-      <c r="B83" s="2" t="s">
-        <v>40</v>
       </c>
       <c r="C83" s="1" t="n">
         <v>6</v>
@@ -1643,16 +1632,16 @@
         <f aca="false">12*13.86</f>
         <v>166.32</v>
       </c>
-      <c r="G83" s="1" t="n">
+      <c r="F83" s="1" t="n">
         <v>0.2016</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B84" s="2" t="s">
         <v>41</v>
-      </c>
-      <c r="B84" s="2" t="s">
-        <v>42</v>
       </c>
       <c r="C84" s="1" t="n">
         <v>3</v>
@@ -1661,16 +1650,16 @@
         <f aca="false">12*11.79</f>
         <v>141.48</v>
       </c>
-      <c r="G84" s="1" t="n">
+      <c r="F84" s="1" t="n">
         <v>0.19522</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B85" s="2" t="s">
         <v>41</v>
-      </c>
-      <c r="B85" s="2" t="s">
-        <v>42</v>
       </c>
       <c r="C85" s="1" t="n">
         <v>6</v>
@@ -1679,16 +1668,16 @@
         <f aca="false">12*15.59</f>
         <v>187.08</v>
       </c>
-      <c r="G85" s="1" t="n">
+      <c r="F85" s="1" t="n">
         <v>0.19522</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B86" s="2" t="s">
         <v>41</v>
-      </c>
-      <c r="B86" s="2" t="s">
-        <v>42</v>
       </c>
       <c r="C86" s="1" t="n">
         <v>9</v>
@@ -1697,16 +1686,16 @@
         <f aca="false">12*19.58</f>
         <v>234.96</v>
       </c>
-      <c r="G86" s="1" t="n">
+      <c r="F86" s="1" t="n">
         <v>0.19522</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B87" s="2" t="s">
         <v>41</v>
-      </c>
-      <c r="B87" s="2" t="s">
-        <v>42</v>
       </c>
       <c r="C87" s="1" t="n">
         <v>12</v>
@@ -1715,16 +1704,16 @@
         <f aca="false">12*23.58</f>
         <v>282.96</v>
       </c>
-      <c r="G87" s="1" t="n">
+      <c r="F87" s="1" t="n">
         <v>0.19522</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B88" s="2" t="s">
         <v>41</v>
-      </c>
-      <c r="B88" s="2" t="s">
-        <v>42</v>
       </c>
       <c r="C88" s="1" t="n">
         <v>15</v>
@@ -1733,16 +1722,16 @@
         <f aca="false">12*27.38</f>
         <v>328.56</v>
       </c>
-      <c r="G88" s="1" t="n">
+      <c r="F88" s="1" t="n">
         <v>0.19522</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B89" s="2" t="s">
         <v>41</v>
-      </c>
-      <c r="B89" s="2" t="s">
-        <v>42</v>
       </c>
       <c r="C89" s="1" t="n">
         <v>18</v>
@@ -1751,16 +1740,16 @@
         <f aca="false">12*31.14</f>
         <v>373.68</v>
       </c>
-      <c r="G89" s="1" t="n">
+      <c r="F89" s="1" t="n">
         <v>0.19522</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B90" s="2" t="s">
         <v>41</v>
-      </c>
-      <c r="B90" s="2" t="s">
-        <v>42</v>
       </c>
       <c r="C90" s="1" t="n">
         <v>24</v>
@@ -1769,16 +1758,16 @@
         <f aca="false">12*39.29</f>
         <v>471.48</v>
       </c>
-      <c r="G90" s="1" t="n">
+      <c r="F90" s="1" t="n">
         <v>0.19522</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B91" s="2" t="s">
         <v>41</v>
-      </c>
-      <c r="B91" s="2" t="s">
-        <v>42</v>
       </c>
       <c r="C91" s="1" t="n">
         <v>30</v>
@@ -1787,16 +1776,16 @@
         <f aca="false">12*47.07</f>
         <v>564.84</v>
       </c>
-      <c r="G91" s="1" t="n">
+      <c r="F91" s="1" t="n">
         <v>0.19522</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B92" s="2" t="s">
         <v>41</v>
-      </c>
-      <c r="B92" s="2" t="s">
-        <v>42</v>
       </c>
       <c r="C92" s="1" t="n">
         <v>36</v>
@@ -1805,89 +1794,179 @@
         <f aca="false">12*55.05</f>
         <v>660.6</v>
       </c>
-      <c r="G92" s="1" t="n">
+      <c r="F92" s="1" t="n">
         <v>0.19522</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A93" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B93" s="2"/>
       <c r="C93" s="1" t="n">
         <v>3</v>
       </c>
+      <c r="D93" s="1" t="n">
+        <v>12.07</v>
+      </c>
+      <c r="E93" s="1" t="n">
+        <f aca="false">IF(D93="","",12*D93)</f>
+        <v>144.84</v>
+      </c>
+      <c r="F93" s="1" t="n">
+        <v>0.19398</v>
+      </c>
     </row>
     <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A94" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B94" s="2"/>
       <c r="C94" s="1" t="n">
         <v>6</v>
       </c>
+      <c r="D94" s="1" t="n">
+        <v>15.74</v>
+      </c>
+      <c r="E94" s="1" t="n">
+        <f aca="false">IF(D94="","",12*D94)</f>
+        <v>188.88</v>
+      </c>
+      <c r="F94" s="1" t="n">
+        <v>0.19398</v>
+      </c>
     </row>
     <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A95" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B95" s="2"/>
       <c r="C95" s="1" t="n">
         <v>9</v>
       </c>
+      <c r="D95" s="1" t="n">
+        <v>19.69</v>
+      </c>
+      <c r="E95" s="1" t="n">
+        <f aca="false">IF(D95="","",12*D95)</f>
+        <v>236.28</v>
+      </c>
+      <c r="F95" s="1" t="n">
+        <v>0.19266</v>
+      </c>
     </row>
     <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A96" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B96" s="2"/>
       <c r="C96" s="1" t="n">
         <v>12</v>
       </c>
+      <c r="D96" s="1" t="n">
+        <v>23.49</v>
+      </c>
+      <c r="E96" s="1" t="n">
+        <f aca="false">IF(D96="","",12*D96)</f>
+        <v>281.88</v>
+      </c>
+      <c r="F96" s="1" t="n">
+        <v>0.19266</v>
+      </c>
     </row>
     <row r="97" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A97" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B97" s="2"/>
       <c r="C97" s="1" t="n">
         <v>15</v>
       </c>
+      <c r="D97" s="1" t="n">
+        <v>27.06</v>
+      </c>
+      <c r="E97" s="1" t="n">
+        <f aca="false">IF(D97="","",12*D97)</f>
+        <v>324.72</v>
+      </c>
+      <c r="F97" s="1" t="n">
+        <v>0.19266</v>
+      </c>
     </row>
     <row r="98" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A98" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B98" s="2"/>
       <c r="C98" s="1" t="n">
         <v>18</v>
       </c>
+      <c r="D98" s="1" t="n">
+        <v>30.75</v>
+      </c>
+      <c r="E98" s="1" t="n">
+        <f aca="false">IF(D98="","",12*D98)</f>
+        <v>369</v>
+      </c>
+      <c r="F98" s="1" t="n">
+        <v>0.19266</v>
+      </c>
     </row>
     <row r="99" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A99" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B99" s="2"/>
       <c r="C99" s="1" t="n">
         <v>24</v>
       </c>
+      <c r="D99" s="1" t="n">
+        <v>38.59</v>
+      </c>
+      <c r="E99" s="1" t="n">
+        <f aca="false">IF(D99="","",12*D99)</f>
+        <v>463.08</v>
+      </c>
+      <c r="F99" s="1" t="n">
+        <v>0.19266</v>
+      </c>
     </row>
     <row r="100" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A100" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B100" s="2"/>
       <c r="C100" s="1" t="n">
         <v>30</v>
       </c>
+      <c r="D100" s="1" t="n">
+        <v>45.8</v>
+      </c>
+      <c r="E100" s="1" t="n">
+        <f aca="false">IF(D100="","",12*D100)</f>
+        <v>549.6</v>
+      </c>
+      <c r="F100" s="1" t="n">
+        <v>0.19266</v>
+      </c>
     </row>
     <row r="101" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A101" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B101" s="2"/>
       <c r="C101" s="1" t="n">
         <v>36</v>
+      </c>
+      <c r="D101" s="1" t="n">
+        <v>53.06</v>
+      </c>
+      <c r="E101" s="1" t="n">
+        <f aca="false">IF(D101="","",12*D101)</f>
+        <v>636.72</v>
+      </c>
+      <c r="F101" s="1" t="n">
+        <v>0.19266</v>
       </c>
     </row>
   </sheetData>

</xml_diff>